<commit_message>
improved verions for pypi
</commit_message>
<xml_diff>
--- a/template/test_set.xlsx
+++ b/template/test_set.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jingyiniu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E756D8E9-A9BA-4540-B361-AAA55970E2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8225A7-39FD-4955-8D31-CADF55BD62A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23596" windowHeight="15076" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="1205" sheetId="1" r:id="rId1"/>
+    <sheet name="query" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1205'!$A$1:$B$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">query!$A$1:$B$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -627,7 +627,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B3"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.78515625" defaultRowHeight="12.75"/>

</xml_diff>